<commit_message>
nieuwe trainingsuren & latest dish
</commit_message>
<xml_diff>
--- a/_content/training/2022/trainingsuren-2022-2023.xlsx
+++ b/_content/training/2022/trainingsuren-2022-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\basket\lummen\_content\training\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAFF5DA9-7CF6-4F59-B4F7-528E91F1B334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0195DB39-1885-439B-8621-A869BE4CB38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Maandag" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="76">
   <si>
     <t>Maandag</t>
   </si>
@@ -217,56 +217,56 @@
     <t>Volleyball</t>
   </si>
   <si>
-    <t>U19+D-B</t>
-  </si>
-  <si>
     <t>M14</t>
   </si>
   <si>
-    <t>M19B</t>
-  </si>
-  <si>
     <t>M19A</t>
   </si>
   <si>
-    <t>M16C</t>
-  </si>
-  <si>
     <t>D-B</t>
   </si>
   <si>
-    <t>U16A+B??</t>
-  </si>
-  <si>
-    <t>M19B Week A</t>
-  </si>
-  <si>
-    <t>M19B Week B</t>
-  </si>
-  <si>
     <t>H-D</t>
   </si>
   <si>
     <t>U12D</t>
   </si>
   <si>
-    <t>U10C/D</t>
-  </si>
-  <si>
     <t>M16A+B</t>
   </si>
   <si>
-    <t>U16??</t>
-  </si>
-  <si>
-    <t>U14Niv2</t>
+    <t>Kolom1</t>
+  </si>
+  <si>
+    <t>Diest</t>
+  </si>
+  <si>
+    <t>Wordt 17:45 - 19:15</t>
+  </si>
+  <si>
+    <t>Wordt 19:00 tot 19:15 (U12 + U14) ieder één 1/2 veld dan switch U12 naar veld om 19:15</t>
+  </si>
+  <si>
+    <t>U14A/U12A</t>
+  </si>
+  <si>
+    <t>U16A+B/U12A</t>
+  </si>
+  <si>
+    <t>U10A/U12C</t>
+  </si>
+  <si>
+    <t>U16</t>
+  </si>
+  <si>
+    <t>Opgelet eerste donderdag van elke maand starten M14 van 17:00 - 18:30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,8 +320,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,8 +385,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF03CD16"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -639,11 +666,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -702,9 +766,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -720,18 +781,9 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -743,15 +795,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -778,6 +821,68 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -797,7 +902,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="39">
     <dxf>
       <font>
         <b val="0"/>
@@ -1939,6 +2044,47 @@
         <vertAlign val="baseline"/>
         <sz val="8"/>
         <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
@@ -2179,6 +2325,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF03CD16"/>
       <color rgb="FFFFFEAB"/>
     </mruColors>
   </colors>
@@ -2194,14 +2341,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabel13" displayName="Tabel13" ref="A2:H29" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
-  <autoFilter ref="A2:H29" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Maandag" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SH1" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="SH2" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SH3" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="OHVM" dataDxfId="31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabel13" displayName="Tabel13" ref="A2:I29" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+  <autoFilter ref="A2:I29" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Maandag" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SH1" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="SH2" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SH3" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="OHVM" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{AC85250E-47DE-450E-AB36-DE1428B6C527}" name="Kolom1" dataDxfId="31"/>
     <tableColumn id="6" xr3:uid="{514B5E76-8E20-49FC-9141-2E662AF77F57}" name="SH12" dataDxfId="30"/>
     <tableColumn id="8" xr3:uid="{74DD8150-5334-4881-B83A-50C88DD527B8}" name="SH23" dataDxfId="29"/>
     <tableColumn id="9" xr3:uid="{D1935B45-1EBF-4BCC-A2D3-59CBB2E1D7A4}" name="SH34" dataDxfId="28"/>
@@ -2553,32 +2701,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:AE58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15:Y53"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="5" width="10" customWidth="1"/>
+    <col min="2" max="6" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="46" t="s">
+    <row r="1" spans="1:31" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="50"/>
-    </row>
-    <row r="2" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="64"/>
+      <c r="I1" s="65"/>
+    </row>
+    <row r="2" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2594,17 +2745,20 @@
       <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2612,11 +2766,12 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-    </row>
-    <row r="4" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="4" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2627,8 +2782,9 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2639,8 +2795,9 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -2651,8 +2808,9 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -2663,8 +2821,9 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2675,8 +2834,9 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -2687,8 +2847,29 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="3"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="42"/>
+      <c r="V9" s="42"/>
+      <c r="W9" s="42"/>
+      <c r="X9" s="42"/>
+      <c r="Y9" s="42"/>
+      <c r="Z9" s="42"/>
+      <c r="AA9" s="42"/>
+      <c r="AB9" s="42"/>
+      <c r="AC9" s="42"/>
+      <c r="AD9" s="42"/>
+      <c r="AE9" s="42"/>
+    </row>
+    <row r="10" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -2699,8 +2880,29 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="3"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="42"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="42"/>
+      <c r="U10" s="42"/>
+      <c r="V10" s="42"/>
+      <c r="W10" s="42"/>
+      <c r="X10" s="42"/>
+      <c r="Y10" s="42"/>
+      <c r="Z10" s="42"/>
+      <c r="AA10" s="42"/>
+      <c r="AB10" s="42"/>
+      <c r="AC10" s="42"/>
+      <c r="AD10" s="42"/>
+      <c r="AE10" s="42"/>
+    </row>
+    <row r="11" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -2711,8 +2913,29 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="3"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="42"/>
+      <c r="V11" s="42"/>
+      <c r="W11" s="42"/>
+      <c r="X11" s="42"/>
+      <c r="Y11" s="42"/>
+      <c r="Z11" s="42"/>
+      <c r="AA11" s="42"/>
+      <c r="AB11" s="42"/>
+      <c r="AC11" s="42"/>
+      <c r="AD11" s="42"/>
+      <c r="AE11" s="42"/>
+    </row>
+    <row r="12" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -2723,8 +2946,29 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="3"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="42"/>
+      <c r="V12" s="42"/>
+      <c r="W12" s="42"/>
+      <c r="X12" s="42"/>
+      <c r="Y12" s="42"/>
+      <c r="Z12" s="42"/>
+      <c r="AA12" s="42"/>
+      <c r="AB12" s="42"/>
+      <c r="AC12" s="42"/>
+      <c r="AD12" s="42"/>
+      <c r="AE12" s="42"/>
+    </row>
+    <row r="13" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -2735,8 +2979,29 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="3"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="42"/>
+      <c r="T13" s="42"/>
+      <c r="U13" s="42"/>
+      <c r="V13" s="42"/>
+      <c r="W13" s="42"/>
+      <c r="X13" s="42"/>
+      <c r="Y13" s="42"/>
+      <c r="Z13" s="42"/>
+      <c r="AA13" s="42"/>
+      <c r="AB13" s="42"/>
+      <c r="AC13" s="42"/>
+      <c r="AD13" s="42"/>
+      <c r="AE13" s="42"/>
+    </row>
+    <row r="14" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -2747,8 +3012,29 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="3"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="42"/>
+      <c r="V14" s="42"/>
+      <c r="W14" s="42"/>
+      <c r="X14" s="42"/>
+      <c r="Y14" s="42"/>
+      <c r="Z14" s="42"/>
+      <c r="AA14" s="42"/>
+      <c r="AB14" s="42"/>
+      <c r="AC14" s="42"/>
+      <c r="AD14" s="42"/>
+      <c r="AE14" s="42"/>
+    </row>
+    <row r="15" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -2759,8 +3045,29 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="3"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="42"/>
+      <c r="V15" s="42"/>
+      <c r="W15" s="42"/>
+      <c r="X15" s="42"/>
+      <c r="Y15" s="42"/>
+      <c r="Z15" s="42"/>
+      <c r="AA15" s="42"/>
+      <c r="AB15" s="42"/>
+      <c r="AC15" s="42"/>
+      <c r="AD15" s="42"/>
+      <c r="AE15" s="42"/>
+    </row>
+    <row r="16" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -2771,206 +3078,440 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="3"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="42"/>
+      <c r="T16" s="42"/>
+      <c r="U16" s="42"/>
+      <c r="V16" s="42"/>
+      <c r="W16" s="42"/>
+      <c r="X16" s="42"/>
+      <c r="Y16" s="42"/>
+      <c r="Z16" s="42"/>
+      <c r="AA16" s="42"/>
+      <c r="AB16" s="42"/>
+      <c r="AC16" s="42"/>
+      <c r="AD16" s="42"/>
+      <c r="AE16" s="42"/>
+    </row>
+    <row r="17" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="38"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="7"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="42"/>
+      <c r="R17" s="42"/>
+      <c r="S17" s="42"/>
+      <c r="T17" s="42"/>
+      <c r="U17" s="42"/>
+      <c r="V17" s="42"/>
+      <c r="W17" s="42"/>
+      <c r="X17" s="42"/>
+      <c r="Y17" s="42"/>
+      <c r="Z17" s="42"/>
+      <c r="AA17" s="42"/>
+      <c r="AB17" s="42"/>
+      <c r="AC17" s="42"/>
+      <c r="AD17" s="42"/>
+      <c r="AE17" s="42"/>
+    </row>
+    <row r="18" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="38"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="7"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="42"/>
+      <c r="S18" s="42"/>
+      <c r="T18" s="42"/>
+      <c r="U18" s="42"/>
+      <c r="V18" s="42"/>
+      <c r="W18" s="42"/>
+      <c r="X18" s="42"/>
+      <c r="Y18" s="42"/>
+      <c r="Z18" s="42"/>
+      <c r="AA18" s="42"/>
+      <c r="AB18" s="42"/>
+      <c r="AC18" s="42"/>
+      <c r="AD18" s="42"/>
+      <c r="AE18" s="42"/>
+    </row>
+    <row r="19" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="16"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="H19" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="47"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="42"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="42"/>
+      <c r="V19" s="42"/>
+      <c r="W19" s="42"/>
+      <c r="X19" s="42"/>
+      <c r="Y19" s="42"/>
+      <c r="Z19" s="42"/>
+      <c r="AA19" s="42"/>
+      <c r="AB19" s="42"/>
+      <c r="AC19" s="42"/>
+      <c r="AD19" s="42"/>
+      <c r="AE19" s="42"/>
+    </row>
+    <row r="20" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="47"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="42"/>
+      <c r="Q20" s="42"/>
+      <c r="R20" s="42"/>
+      <c r="S20" s="42"/>
+      <c r="T20" s="42"/>
+      <c r="U20" s="42"/>
+      <c r="V20" s="42"/>
+      <c r="W20" s="42"/>
+      <c r="X20" s="42"/>
+      <c r="Y20" s="42"/>
+      <c r="Z20" s="42"/>
+      <c r="AA20" s="42"/>
+      <c r="AB20" s="42"/>
+      <c r="AC20" s="42"/>
+      <c r="AD20" s="42"/>
+      <c r="AE20" s="42"/>
+    </row>
+    <row r="21" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="39" t="s">
+      <c r="E21" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="39" t="s">
+      <c r="H21" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="H21" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="47"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="42"/>
+      <c r="S21" s="42"/>
+      <c r="T21" s="42"/>
+      <c r="U21" s="42"/>
+      <c r="V21" s="42"/>
+      <c r="W21" s="42"/>
+      <c r="X21" s="42"/>
+      <c r="Y21" s="42"/>
+      <c r="Z21" s="42"/>
+      <c r="AA21" s="42"/>
+      <c r="AB21" s="42"/>
+      <c r="AC21" s="42"/>
+      <c r="AD21" s="42"/>
+      <c r="AE21" s="42"/>
+    </row>
+    <row r="22" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="16"/>
-      <c r="C22" s="33"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="39" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="6"/>
+      <c r="G22" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" s="47"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="42"/>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="42"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="42"/>
+      <c r="U22" s="42"/>
+      <c r="V22" s="42"/>
+      <c r="W22" s="42"/>
+      <c r="X22" s="42"/>
+      <c r="Y22" s="42"/>
+      <c r="Z22" s="42"/>
+      <c r="AA22" s="42"/>
+      <c r="AB22" s="42"/>
+      <c r="AC22" s="42"/>
+      <c r="AD22" s="42"/>
+      <c r="AE22" s="42"/>
+    </row>
+    <row r="23" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="24" t="s">
+      <c r="B23" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E23" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" s="39" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="4"/>
+      <c r="G23" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="47"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="42"/>
+      <c r="Q23" s="42"/>
+      <c r="R23" s="42"/>
+      <c r="S23" s="42"/>
+      <c r="T23" s="42"/>
+      <c r="U23" s="42"/>
+      <c r="V23" s="42"/>
+      <c r="W23" s="42"/>
+      <c r="X23" s="42"/>
+      <c r="Y23" s="42"/>
+      <c r="Z23" s="42"/>
+      <c r="AA23" s="42"/>
+      <c r="AB23" s="42"/>
+      <c r="AC23" s="42"/>
+      <c r="AD23" s="42"/>
+      <c r="AE23" s="42"/>
+    </row>
+    <row r="24" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="24" t="s">
+      <c r="B24" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="E24" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="G24" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="H24" s="39" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="4"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="47"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="42"/>
+      <c r="S24" s="42"/>
+      <c r="T24" s="42"/>
+      <c r="U24" s="42"/>
+      <c r="V24" s="42"/>
+      <c r="W24" s="42"/>
+      <c r="X24" s="42"/>
+      <c r="Y24" s="42"/>
+      <c r="Z24" s="42"/>
+      <c r="AA24" s="42"/>
+      <c r="AB24" s="42"/>
+      <c r="AC24" s="42"/>
+      <c r="AD24" s="42"/>
+      <c r="AE24" s="42"/>
+    </row>
+    <row r="25" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="24" t="s">
+      <c r="B25" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="39" t="s">
         <v>25</v>
       </c>
       <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="F25" s="50" t="s">
+        <v>62</v>
+      </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="6"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="42"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="42"/>
+      <c r="U25" s="42"/>
+      <c r="V25" s="42"/>
+      <c r="W25" s="42"/>
+      <c r="X25" s="42"/>
+      <c r="Y25" s="42"/>
+      <c r="Z25" s="42"/>
+      <c r="AA25" s="42"/>
+      <c r="AB25" s="42"/>
+      <c r="AC25" s="42"/>
+      <c r="AD25" s="42"/>
+      <c r="AE25" s="42"/>
+    </row>
+    <row r="26" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="16"/>
-      <c r="C26" s="33"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+      <c r="F26" s="50" t="s">
+        <v>62</v>
+      </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="6"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="42"/>
+      <c r="S26" s="42"/>
+      <c r="T26" s="42"/>
+      <c r="U26" s="42"/>
+      <c r="V26" s="42"/>
+      <c r="W26" s="42"/>
+      <c r="X26" s="42"/>
+      <c r="Y26" s="42"/>
+      <c r="Z26" s="42"/>
+      <c r="AA26" s="42"/>
+      <c r="AB26" s="42"/>
+      <c r="AC26" s="42"/>
+      <c r="AD26" s="42"/>
+      <c r="AE26" s="42"/>
+    </row>
+    <row r="27" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="16"/>
-      <c r="C27" s="33"/>
+      <c r="C27" s="29"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="50" t="s">
+        <v>62</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="4"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="42"/>
+      <c r="S27" s="42"/>
+      <c r="T27" s="42"/>
+      <c r="U27" s="42"/>
+      <c r="V27" s="42"/>
+      <c r="W27" s="42"/>
+      <c r="X27" s="42"/>
+      <c r="Y27" s="42"/>
+      <c r="Z27" s="42"/>
+      <c r="AA27" s="42"/>
+      <c r="AB27" s="42"/>
+      <c r="AC27" s="42"/>
+      <c r="AD27" s="42"/>
+      <c r="AE27" s="42"/>
+    </row>
+    <row r="28" spans="1:31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -2978,11 +3519,34 @@
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="50" t="s">
+        <v>62</v>
+      </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I28" s="4"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="42"/>
+      <c r="Q28" s="42"/>
+      <c r="R28" s="42"/>
+      <c r="S28" s="42"/>
+      <c r="T28" s="42"/>
+      <c r="U28" s="42"/>
+      <c r="V28" s="42"/>
+      <c r="W28" s="42"/>
+      <c r="X28" s="42"/>
+      <c r="Y28" s="42"/>
+      <c r="Z28" s="42"/>
+      <c r="AA28" s="42"/>
+      <c r="AB28" s="42"/>
+      <c r="AC28" s="42"/>
+      <c r="AD28" s="42"/>
+      <c r="AE28" s="42"/>
+    </row>
+    <row r="29" spans="1:31" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -2990,41 +3554,505 @@
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
       <c r="E29" s="19"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="42"/>
+      <c r="Q29" s="42"/>
+      <c r="R29" s="42"/>
+      <c r="S29" s="42"/>
+      <c r="T29" s="42"/>
+      <c r="U29" s="42"/>
+      <c r="V29" s="42"/>
+      <c r="W29" s="42"/>
+      <c r="X29" s="42"/>
+      <c r="Y29" s="42"/>
+      <c r="Z29" s="42"/>
+      <c r="AA29" s="42"/>
+      <c r="AB29" s="42"/>
+      <c r="AC29" s="42"/>
+      <c r="AD29" s="42"/>
+      <c r="AE29" s="42"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="42"/>
+      <c r="Q30" s="42"/>
+      <c r="R30" s="42"/>
+      <c r="S30" s="42"/>
+      <c r="T30" s="42"/>
+      <c r="U30" s="42"/>
+      <c r="V30" s="42"/>
+      <c r="W30" s="42"/>
+      <c r="X30" s="42"/>
+      <c r="Y30" s="42"/>
+      <c r="Z30" s="42"/>
+      <c r="AA30" s="42"/>
+      <c r="AB30" s="42"/>
+      <c r="AC30" s="42"/>
+      <c r="AD30" s="42"/>
+      <c r="AE30" s="42"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="44"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="42"/>
+      <c r="Q31" s="42"/>
+      <c r="R31" s="42"/>
+      <c r="S31" s="42"/>
+      <c r="T31" s="42"/>
+      <c r="U31" s="42"/>
+      <c r="V31" s="42"/>
+      <c r="W31" s="42"/>
+      <c r="X31" s="42"/>
+      <c r="Y31" s="42"/>
+      <c r="Z31" s="42"/>
+      <c r="AA31" s="42"/>
+      <c r="AB31" s="42"/>
+      <c r="AC31" s="42"/>
+      <c r="AD31" s="42"/>
+      <c r="AE31" s="42"/>
+    </row>
+    <row r="32" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L32" s="42"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="42"/>
+      <c r="Q32" s="42"/>
+      <c r="R32" s="42"/>
+      <c r="S32" s="42"/>
+      <c r="T32" s="42"/>
+      <c r="U32" s="42"/>
+      <c r="V32" s="42"/>
+      <c r="W32" s="42"/>
+      <c r="X32" s="42"/>
+      <c r="Y32" s="42"/>
+      <c r="Z32" s="42"/>
+      <c r="AA32" s="42"/>
+      <c r="AB32" s="42"/>
+      <c r="AC32" s="42"/>
+      <c r="AD32" s="42"/>
+      <c r="AE32" s="42"/>
+    </row>
+    <row r="33" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L33" s="42"/>
+      <c r="M33" s="42"/>
+      <c r="N33" s="44"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="42"/>
+      <c r="Q33" s="42"/>
+      <c r="R33" s="42"/>
+      <c r="S33" s="42"/>
+      <c r="T33" s="42"/>
+      <c r="U33" s="42"/>
+      <c r="V33" s="42"/>
+      <c r="W33" s="42"/>
+      <c r="X33" s="42"/>
+      <c r="Y33" s="42"/>
+      <c r="Z33" s="42"/>
+      <c r="AA33" s="42"/>
+      <c r="AB33" s="42"/>
+      <c r="AC33" s="42"/>
+      <c r="AD33" s="42"/>
+      <c r="AE33" s="42"/>
+    </row>
+    <row r="34" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L34" s="42"/>
+      <c r="M34" s="42"/>
+      <c r="N34" s="44"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="42"/>
+      <c r="Q34" s="42"/>
+      <c r="R34" s="42"/>
+      <c r="S34" s="42"/>
+      <c r="T34" s="42"/>
+      <c r="U34" s="42"/>
+      <c r="V34" s="42"/>
+      <c r="W34" s="42"/>
+      <c r="X34" s="42"/>
+      <c r="Y34" s="42"/>
+      <c r="Z34" s="42"/>
+      <c r="AA34" s="42"/>
+      <c r="AB34" s="42"/>
+      <c r="AC34" s="42"/>
+      <c r="AD34" s="42"/>
+      <c r="AE34" s="42"/>
+    </row>
+    <row r="35" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L35" s="42"/>
+      <c r="M35" s="42"/>
+      <c r="N35" s="44"/>
+      <c r="O35" s="42"/>
+      <c r="P35" s="42"/>
+      <c r="Q35" s="42"/>
+      <c r="R35" s="42"/>
+      <c r="S35" s="42"/>
+      <c r="T35" s="42"/>
+      <c r="U35" s="42"/>
+      <c r="V35" s="42"/>
+      <c r="W35" s="42"/>
+      <c r="X35" s="42"/>
+      <c r="Y35" s="42"/>
+      <c r="Z35" s="42"/>
+      <c r="AA35" s="42"/>
+      <c r="AB35" s="42"/>
+      <c r="AC35" s="42"/>
+      <c r="AD35" s="42"/>
+      <c r="AE35" s="42"/>
+    </row>
+    <row r="36" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L36" s="42"/>
+      <c r="M36" s="42"/>
+      <c r="N36" s="44"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="42"/>
+      <c r="Q36" s="42"/>
+      <c r="R36" s="42"/>
+      <c r="S36" s="42"/>
+      <c r="T36" s="42"/>
+      <c r="U36" s="42"/>
+      <c r="V36" s="42"/>
+      <c r="W36" s="42"/>
+      <c r="X36" s="42"/>
+      <c r="Y36" s="42"/>
+      <c r="Z36" s="42"/>
+      <c r="AA36" s="42"/>
+      <c r="AB36" s="42"/>
+      <c r="AC36" s="42"/>
+      <c r="AD36" s="42"/>
+      <c r="AE36" s="42"/>
+    </row>
+    <row r="37" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L37" s="42"/>
+      <c r="M37" s="42"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="42"/>
+      <c r="Q37" s="42"/>
+      <c r="R37" s="42"/>
+      <c r="S37" s="42"/>
+      <c r="T37" s="42"/>
+      <c r="U37" s="42"/>
+      <c r="V37" s="42"/>
+      <c r="W37" s="42"/>
+      <c r="X37" s="42"/>
+      <c r="Y37" s="42"/>
+      <c r="Z37" s="42"/>
+      <c r="AA37" s="42"/>
+      <c r="AB37" s="42"/>
+      <c r="AC37" s="42"/>
+      <c r="AD37" s="42"/>
+      <c r="AE37" s="42"/>
+    </row>
+    <row r="38" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L38" s="42"/>
+      <c r="M38" s="42"/>
+      <c r="N38" s="44"/>
+      <c r="O38" s="42"/>
+      <c r="P38" s="42"/>
+      <c r="Q38" s="42"/>
+      <c r="R38" s="42"/>
+      <c r="S38" s="42"/>
+      <c r="T38" s="42"/>
+      <c r="U38" s="42"/>
+      <c r="V38" s="42"/>
+      <c r="W38" s="42"/>
+      <c r="X38" s="42"/>
+      <c r="Y38" s="42"/>
+      <c r="Z38" s="42"/>
+      <c r="AA38" s="42"/>
+      <c r="AB38" s="42"/>
+      <c r="AC38" s="42"/>
+      <c r="AD38" s="42"/>
+      <c r="AE38" s="42"/>
+    </row>
+    <row r="39" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L39" s="42"/>
+      <c r="M39" s="42"/>
+      <c r="N39" s="44"/>
+      <c r="O39" s="42"/>
+      <c r="P39" s="42"/>
+      <c r="Q39" s="42"/>
+      <c r="R39" s="42"/>
+      <c r="S39" s="42"/>
+      <c r="T39" s="42"/>
+      <c r="U39" s="42"/>
+      <c r="V39" s="42"/>
+      <c r="W39" s="42"/>
+      <c r="X39" s="42"/>
+      <c r="Y39" s="42"/>
+      <c r="Z39" s="42"/>
+      <c r="AA39" s="42"/>
+      <c r="AB39" s="42"/>
+      <c r="AC39" s="42"/>
+      <c r="AD39" s="42"/>
+      <c r="AE39" s="42"/>
+    </row>
+    <row r="40" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L40" s="42"/>
+      <c r="M40" s="42"/>
+      <c r="N40" s="45"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="42"/>
+      <c r="Q40" s="42"/>
+      <c r="R40" s="42"/>
+      <c r="S40" s="42"/>
+      <c r="T40" s="42"/>
+      <c r="U40" s="42"/>
+      <c r="V40" s="42"/>
+      <c r="W40" s="42"/>
+      <c r="X40" s="42"/>
+      <c r="Y40" s="42"/>
+      <c r="Z40" s="42"/>
+      <c r="AA40" s="42"/>
+      <c r="AB40" s="42"/>
+      <c r="AC40" s="42"/>
+      <c r="AD40" s="42"/>
+      <c r="AE40" s="42"/>
+    </row>
+    <row r="41" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L41" s="42"/>
+      <c r="M41" s="42"/>
+      <c r="N41" s="44"/>
+      <c r="O41" s="42"/>
+      <c r="P41" s="42"/>
+      <c r="Q41" s="42"/>
+      <c r="R41" s="42"/>
+      <c r="S41" s="42"/>
+      <c r="T41" s="42"/>
+      <c r="U41" s="42"/>
+      <c r="V41" s="42"/>
+      <c r="W41" s="42"/>
+      <c r="X41" s="42"/>
+      <c r="Y41" s="42"/>
+      <c r="Z41" s="42"/>
+      <c r="AA41" s="42"/>
+      <c r="AB41" s="42"/>
+      <c r="AC41" s="42"/>
+      <c r="AD41" s="42"/>
+      <c r="AE41" s="42"/>
+    </row>
+    <row r="42" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L42" s="42"/>
+      <c r="M42" s="42"/>
+      <c r="N42" s="44"/>
+      <c r="O42" s="42"/>
+      <c r="P42" s="42"/>
+      <c r="Q42" s="42"/>
+      <c r="R42" s="42"/>
+      <c r="S42" s="42"/>
+      <c r="T42" s="42"/>
+      <c r="U42" s="42"/>
+      <c r="V42" s="42"/>
+      <c r="W42" s="42"/>
+      <c r="X42" s="42"/>
+      <c r="Y42" s="42"/>
+      <c r="Z42" s="42"/>
+      <c r="AA42" s="42"/>
+      <c r="AB42" s="42"/>
+      <c r="AC42" s="42"/>
+      <c r="AD42" s="42"/>
+      <c r="AE42" s="42"/>
+    </row>
+    <row r="43" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L43" s="42"/>
+      <c r="M43" s="42"/>
+      <c r="N43" s="44"/>
+      <c r="O43" s="42"/>
+      <c r="P43" s="42"/>
+      <c r="Q43" s="42"/>
+      <c r="R43" s="42"/>
+      <c r="S43" s="42"/>
+      <c r="T43" s="42"/>
+      <c r="U43" s="42"/>
+      <c r="V43" s="42"/>
+      <c r="W43" s="42"/>
+      <c r="X43" s="42"/>
+      <c r="Y43" s="42"/>
+      <c r="Z43" s="42"/>
+      <c r="AA43" s="42"/>
+      <c r="AB43" s="42"/>
+      <c r="AC43" s="42"/>
+      <c r="AD43" s="42"/>
+      <c r="AE43" s="42"/>
+    </row>
+    <row r="44" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L44" s="42"/>
+      <c r="M44" s="42"/>
+      <c r="N44" s="43"/>
+      <c r="O44" s="42"/>
+      <c r="P44" s="42"/>
+      <c r="Q44" s="42"/>
+      <c r="R44" s="42"/>
+      <c r="S44" s="42"/>
+      <c r="T44" s="42"/>
+      <c r="U44" s="42"/>
+      <c r="V44" s="42"/>
+      <c r="W44" s="42"/>
+      <c r="X44" s="42"/>
+      <c r="Y44" s="42"/>
+      <c r="Z44" s="42"/>
+      <c r="AA44" s="42"/>
+      <c r="AB44" s="42"/>
+      <c r="AC44" s="42"/>
+      <c r="AD44" s="42"/>
+      <c r="AE44" s="42"/>
+    </row>
+    <row r="45" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L45" s="42"/>
+      <c r="M45" s="42"/>
+      <c r="N45" s="44"/>
+      <c r="O45" s="42"/>
+      <c r="P45" s="42"/>
+      <c r="Q45" s="42"/>
+      <c r="R45" s="42"/>
+      <c r="S45" s="42"/>
+      <c r="T45" s="42"/>
+      <c r="U45" s="42"/>
+      <c r="V45" s="42"/>
+      <c r="W45" s="42"/>
+      <c r="X45" s="42"/>
+      <c r="Y45" s="42"/>
+      <c r="Z45" s="42"/>
+      <c r="AA45" s="42"/>
+      <c r="AB45" s="42"/>
+      <c r="AC45" s="42"/>
+      <c r="AD45" s="42"/>
+      <c r="AE45" s="42"/>
+    </row>
+    <row r="46" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L46" s="42"/>
+      <c r="M46" s="42"/>
+      <c r="N46" s="44"/>
+      <c r="O46" s="42"/>
+      <c r="P46" s="42"/>
+      <c r="Q46" s="42"/>
+      <c r="R46" s="42"/>
+      <c r="S46" s="42"/>
+      <c r="T46" s="42"/>
+      <c r="U46" s="42"/>
+      <c r="V46" s="42"/>
+      <c r="W46" s="42"/>
+      <c r="X46" s="42"/>
+      <c r="Y46" s="42"/>
+      <c r="Z46" s="42"/>
+      <c r="AA46" s="42"/>
+      <c r="AB46" s="42"/>
+      <c r="AC46" s="42"/>
+      <c r="AD46" s="42"/>
+      <c r="AE46" s="42"/>
+    </row>
+    <row r="47" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L47" s="42"/>
+      <c r="M47" s="42"/>
+      <c r="N47" s="44"/>
+      <c r="O47" s="42"/>
+      <c r="P47" s="42"/>
+      <c r="Q47" s="42"/>
+      <c r="R47" s="42"/>
+      <c r="S47" s="42"/>
+      <c r="T47" s="42"/>
+      <c r="U47" s="42"/>
+      <c r="V47" s="42"/>
+      <c r="W47" s="42"/>
+      <c r="X47" s="42"/>
+      <c r="Y47" s="42"/>
+      <c r="Z47" s="42"/>
+      <c r="AA47" s="42"/>
+      <c r="AB47" s="42"/>
+      <c r="AC47" s="42"/>
+      <c r="AD47" s="42"/>
+      <c r="AE47" s="42"/>
+    </row>
+    <row r="48" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L48" s="42"/>
+      <c r="M48" s="42"/>
+      <c r="N48" s="42"/>
+      <c r="O48" s="42"/>
+      <c r="P48" s="42"/>
+      <c r="Q48" s="42"/>
+      <c r="R48" s="42"/>
+      <c r="S48" s="42"/>
+      <c r="T48" s="42"/>
+      <c r="U48" s="42"/>
+      <c r="V48" s="42"/>
+      <c r="W48" s="42"/>
+      <c r="X48" s="42"/>
+      <c r="Y48" s="42"/>
+      <c r="Z48" s="42"/>
+      <c r="AA48" s="42"/>
+      <c r="AB48" s="42"/>
+      <c r="AC48" s="42"/>
+      <c r="AD48" s="42"/>
+      <c r="AE48" s="42"/>
+    </row>
+    <row r="49" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L49" s="42"/>
+      <c r="M49" s="42"/>
+      <c r="N49" s="42"/>
+      <c r="O49" s="42"/>
+      <c r="P49" s="42"/>
+      <c r="Q49" s="42"/>
+      <c r="R49" s="42"/>
+      <c r="S49" s="42"/>
+      <c r="T49" s="42"/>
+      <c r="U49" s="42"/>
+      <c r="V49" s="42"/>
+      <c r="W49" s="42"/>
+      <c r="X49" s="42"/>
+      <c r="Y49" s="42"/>
+      <c r="Z49" s="42"/>
+      <c r="AA49" s="42"/>
+      <c r="AB49" s="42"/>
+      <c r="AC49" s="42"/>
+      <c r="AD49" s="42"/>
+      <c r="AE49" s="42"/>
+    </row>
+    <row r="50" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L50" s="42"/>
+      <c r="M50" s="42"/>
+      <c r="N50" s="42"/>
+      <c r="O50" s="42"/>
+      <c r="P50" s="42"/>
+      <c r="Q50" s="42"/>
+      <c r="R50" s="42"/>
+      <c r="S50" s="42"/>
+      <c r="T50" s="42"/>
+      <c r="U50" s="42"/>
+      <c r="V50" s="42"/>
+      <c r="W50" s="42"/>
+      <c r="X50" s="42"/>
+      <c r="Y50" s="42"/>
+      <c r="Z50" s="42"/>
+      <c r="AA50" s="42"/>
+      <c r="AB50" s="42"/>
+      <c r="AC50" s="42"/>
+      <c r="AD50" s="42"/>
+      <c r="AE50" s="42"/>
+    </row>
+    <row r="51" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="12:31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="G1:I1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3039,8 +4067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3049,17 +4077,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="50"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="65"/>
     </row>
     <row r="2" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3095,9 +4123,9 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -3280,7 +4308,7 @@
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="51" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="6"/>
@@ -3292,85 +4320,87 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="51" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="C20" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
     </row>
     <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="51" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="6"/>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="8"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="8"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+    </row>
+    <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="23" t="s">
         <v>51</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>50</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="4"/>
@@ -3378,17 +4408,17 @@
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="24" t="s">
+      <c r="B25" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="23" t="s">
         <v>51</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>50</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="4"/>
@@ -3396,16 +4426,16 @@
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="21" t="s">
+      <c r="B26" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="41" t="s">
         <v>34</v>
       </c>
       <c r="E26" s="8"/>
@@ -3414,16 +4444,16 @@
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="21" t="s">
+      <c r="B27" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="41" t="s">
         <v>34</v>
       </c>
       <c r="E27" s="8"/>
@@ -3432,14 +4462,14 @@
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="21" t="s">
+      <c r="B28" s="53"/>
+      <c r="C28" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="41" t="s">
         <v>34</v>
       </c>
       <c r="E28" s="8"/>
@@ -3448,16 +4478,16 @@
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="36"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="54"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3478,7 +4508,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3487,17 +4517,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="50"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="65"/>
     </row>
     <row r="2" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3533,9 +4563,9 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -3733,13 +4763,13 @@
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="32" t="s">
         <v>56</v>
       </c>
       <c r="E20" s="6"/>
@@ -3751,23 +4781,23 @@
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="32" t="s">
         <v>56</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="F21" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="39" t="s">
+      <c r="F21" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="H21" s="24" t="s">
+      <c r="H21" s="23" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3775,23 +4805,23 @@
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="D22" s="32" t="s">
         <v>56</v>
       </c>
       <c r="E22" s="6"/>
-      <c r="F22" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="39" t="s">
+      <c r="F22" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="24" t="s">
+      <c r="H22" s="23" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3799,23 +4829,21 @@
       <c r="A23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="39" t="s">
+      <c r="B23" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="C23" s="32"/>
+      <c r="D23" s="26" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="6"/>
-      <c r="F23" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="39" t="s">
+      <c r="F23" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="H23" s="24" t="s">
+      <c r="H23" s="23" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3823,13 +4851,11 @@
       <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="39" t="s">
+      <c r="B24" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="C24" s="32"/>
+      <c r="D24" s="26" t="s">
         <v>48</v>
       </c>
       <c r="E24" s="6"/>
@@ -3841,13 +4867,11 @@
       <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="39" t="s">
+      <c r="B25" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="C25" s="32"/>
+      <c r="D25" s="26" t="s">
         <v>48</v>
       </c>
       <c r="E25" s="6"/>
@@ -3859,13 +4883,13 @@
       <c r="A26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="39" t="s">
         <v>25</v>
       </c>
       <c r="E26" s="6"/>
@@ -3877,13 +4901,13 @@
       <c r="A27" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="39" t="s">
         <v>25</v>
       </c>
       <c r="E27" s="6"/>
@@ -3895,13 +4919,13 @@
       <c r="A28" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D28" s="39" t="s">
         <v>25</v>
       </c>
       <c r="E28" s="6"/>
@@ -3913,15 +4937,15 @@
       <c r="A29" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="24" t="s">
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="39" t="s">
         <v>25</v>
       </c>
       <c r="E29" s="7"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
     </row>
     <row r="30" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3940,10 +4964,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="101" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView topLeftCell="A10" zoomScale="101" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3952,17 +4976,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="50"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="65"/>
     </row>
     <row r="2" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3998,9 +5022,9 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -4158,7 +5182,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -4170,7 +5194,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -4182,125 +5206,128 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
-      <c r="E19" s="24" t="s">
-        <v>62</v>
-      </c>
+      <c r="E19" s="32"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="24" t="s">
-        <v>62</v>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="57" t="s">
+        <v>61</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="24" t="s">
+      <c r="C21" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+    </row>
+    <row r="22" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="24" t="s">
+      <c r="C22" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="20" t="s">
-        <v>75</v>
+      <c r="E22" s="57" t="s">
+        <v>61</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="24" t="s">
+      <c r="B23" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="20" t="s">
-        <v>75</v>
+      <c r="E23" s="23" t="s">
+        <v>74</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="24" t="s">
+      <c r="B24" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="20" t="s">
-        <v>75</v>
+      <c r="E24" s="23" t="s">
+        <v>74</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="24" t="s">
+      <c r="B25" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="39" t="s">
         <v>25</v>
       </c>
       <c r="E25" s="10"/>
@@ -4308,17 +5335,17 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="30" t="s">
+      <c r="B26" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="39" t="s">
         <v>25</v>
       </c>
       <c r="E26" s="10"/>
@@ -4326,17 +5353,17 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="30" t="s">
+      <c r="C27" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="40" t="s">
         <v>34</v>
       </c>
       <c r="E27" s="11"/>
@@ -4344,17 +5371,17 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="30" t="s">
+      <c r="C28" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="40" t="s">
         <v>34</v>
       </c>
       <c r="E28" s="11"/>
@@ -4362,21 +5389,21 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="45"/>
+      <c r="C29" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="38"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4396,8 +5423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4406,17 +5433,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="50"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="65"/>
     </row>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4452,9 +5479,9 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -4604,84 +5631,84 @@
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="43"/>
+      <c r="I16" s="36"/>
     </row>
     <row r="17" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="42"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="43"/>
+      <c r="I17" s="36"/>
     </row>
     <row r="18" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="33"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="43"/>
+      <c r="I18" s="36"/>
     </row>
     <row r="19" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="22" t="s">
         <v>36</v>
       </c>
       <c r="E19" s="6"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="43"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="36"/>
     </row>
     <row r="20" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="20" t="s">
         <v>36</v>
       </c>
       <c r="E20" s="6"/>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="39" t="s">
+      <c r="G20" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="39" t="s">
+      <c r="H20" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="I20" s="43"/>
+      <c r="I20" s="36"/>
     </row>
     <row r="21" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -4690,23 +5717,23 @@
       <c r="B21" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="27" t="s">
+      <c r="C21" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="25" t="s">
         <v>57</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="F21" s="39" t="s">
+      <c r="F21" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="39" t="s">
+      <c r="G21" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="39" t="s">
+      <c r="H21" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="I21" s="43"/>
+      <c r="I21" s="36"/>
     </row>
     <row r="22" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -4715,25 +5742,25 @@
       <c r="B22" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="27" t="s">
+      <c r="C22" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="G22" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="H22" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="I22" s="43"/>
+      <c r="G22" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" s="36"/>
     </row>
     <row r="23" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -4742,177 +5769,173 @@
       <c r="B23" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="27" t="s">
+      <c r="C23" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="I23" s="43"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="36"/>
     </row>
     <row r="24" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="30" t="s">
+      <c r="B24" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="I24" s="43"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="36"/>
     </row>
     <row r="25" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="30" t="s">
+      <c r="B25" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="40" t="s">
         <v>46</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="43"/>
+      <c r="I25" s="36"/>
     </row>
     <row r="26" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="30" t="s">
+      <c r="B26" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="40" t="s">
         <v>46</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
-      <c r="I26" s="43"/>
+      <c r="I26" s="36"/>
     </row>
     <row r="27" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="44" t="s">
+      <c r="B27" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="44" t="s">
+      <c r="D27" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="40" t="s">
         <v>46</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
-      <c r="I27" s="43"/>
+      <c r="I27" s="36"/>
     </row>
     <row r="28" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="44" t="s">
+      <c r="D28" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="40" t="s">
         <v>46</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
-      <c r="I28" s="43"/>
+      <c r="I28" s="36"/>
     </row>
     <row r="29" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="44" t="s">
+      <c r="C29" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="33" t="s">
         <v>59</v>
       </c>
       <c r="E29" s="7"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="43"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="36"/>
     </row>
     <row r="30" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>